<commit_message>
Add datasetname slot to Dataset class
</commit_message>
<xml_diff>
--- a/project/excel/brc_schema.xlsx
+++ b/project/excel/brc_schema.xlsx
@@ -444,7 +444,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,6 +511,11 @@
       <c r="L1" t="inlineStr">
         <is>
           <t>keywords</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>datasetname</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Set schema version; update artifacts
</commit_message>
<xml_diff>
--- a/project/excel/brc_schema.xlsx
+++ b/project/excel/brc_schema.xlsx
@@ -444,7 +444,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,30 +495,35 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
+          <t>has_related_ids</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
           <t>species</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>analysisType</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>relatedItem</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>datasetName</t>
         </is>

</xml_diff>

<commit_message>
Add additional_brcs slot to Dataset class
</commit_message>
<xml_diff>
--- a/project/excel/brc_schema.xlsx
+++ b/project/excel/brc_schema.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,76 +481,84 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>additional_brcs</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>repository</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>bibliographicCitation</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>has_related_ids</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>species</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>analysisType</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>datasetType</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>relatedItem</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>datasetName</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>funding</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>dataset_url</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"CABBI,CBI,GLBRC,JBEI"</formula1>
     </dataValidation>
-    <dataValidation sqref="L2:L1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"CABBI,CBI,GLBRC,JBEI"</formula1>
+    </dataValidation>
+    <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"AS,GD,IM,ND,IP,FP,SM,MM,I"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Import OSTI schema within BRC schema; generate artifacts
</commit_message>
<xml_diff>
--- a/project/excel/brc_schema.xlsx
+++ b/project/excel/brc_schema.xlsx
@@ -7,15 +7,28 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="DatasetCollection" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Dataset" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Individual" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Contributor" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Funding" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Organization" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Organism" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Plasmid" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="RelatedItem" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="records" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Record" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="RelatedIdentifier" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Geolocation" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="point" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Identifier" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="AuditLog" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="MediaSet" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="MediaFile" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Organization" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="OrganizationIdentifier" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Person" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Affiliation" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="DatasetCollection" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="Dataset" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="Individual" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="Contributor" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="Funding" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="BRCOrganization" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="Organism" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="Plasmid" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="RelatedItem" sheetId="22" state="visible" r:id="rId22"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -421,6 +434,83 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>records</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>contributor_type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>ror_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>identifiers</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"AUTHOR,CONTRIBUTING,RESEARCHING,SPONSOR"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -432,6 +522,149 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"AWARD_DOI,CN_DOE,CN_NONDOE"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>first_name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>middle_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>last_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>orcid</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>phone</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>osti_user_id</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>contributor_type</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>affiliations</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"AUTHOR,RELEASE,CONTACT,CONTRIBUTING,PROT_CE,PROT_RO,SBIZ_PI,SBIZ_BO"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>ror_id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>datasets</t>
         </is>
       </c>
@@ -446,7 +679,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -593,7 +826,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -639,7 +872,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -690,7 +923,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -731,7 +964,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -772,7 +1005,482 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:CJ1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>osti_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>identifiers</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>issue</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>journal_license_url</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>journal_name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>journal_open_access_flag</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>journal_type</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>revision</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>workflow_status</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>access_limitations</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>access_limitation_other</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>added_by</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>added_by_email</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>added_by_name</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>announcement_codes</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>edition</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>volume</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>collection_type</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>conference_information</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>conference_type</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>contract_award_date</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>country_publication_code</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>date_metadata_added</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>date_metadata_updated</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>date_submitted_to_osti_first</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>date_submitted_to_osti_last</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>descriptors</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>doe_funded_flag</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>doi</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>doi_infix</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>edited_by</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>edited_by_email</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>edited_by_name</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>edit_reason</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>edit_source</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>format_information</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>media_embargo_sunset_date</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>publication_date</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>publication_date_text</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>publisher_information</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>related_doc_info</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>keywords</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>languages</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>audit_logs</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>media</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>opn_addressee</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>opn_declassified_date</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>opn_declassified_status</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>opn_document_categories</t>
+        </is>
+      </c>
+      <c r="AZ1" t="inlineStr">
+        <is>
+          <t>opn_document_location</t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
+          <t>opn_fieldoffice_acronym_code</t>
+        </is>
+      </c>
+      <c r="BB1" t="inlineStr">
+        <is>
+          <t>organizations</t>
+        </is>
+      </c>
+      <c r="BC1" t="inlineStr">
+        <is>
+          <t>other_information</t>
+        </is>
+      </c>
+      <c r="BD1" t="inlineStr">
+        <is>
+          <t>ouo_release_date</t>
+        </is>
+      </c>
+      <c r="BE1" t="inlineStr">
+        <is>
+          <t>paper_flag</t>
+        </is>
+      </c>
+      <c r="BF1" t="inlineStr">
+        <is>
+          <t>patent_assignee</t>
+        </is>
+      </c>
+      <c r="BG1" t="inlineStr">
+        <is>
+          <t>patent_file_date</t>
+        </is>
+      </c>
+      <c r="BH1" t="inlineStr">
+        <is>
+          <t>patent_priority_date</t>
+        </is>
+      </c>
+      <c r="BI1" t="inlineStr">
+        <is>
+          <t>pdouo_exemption_number</t>
+        </is>
+      </c>
+      <c r="BJ1" t="inlineStr">
+        <is>
+          <t>persons</t>
+        </is>
+      </c>
+      <c r="BK1" t="inlineStr">
+        <is>
+          <t>product_size</t>
+        </is>
+      </c>
+      <c r="BL1" t="inlineStr">
+        <is>
+          <t>product_type</t>
+        </is>
+      </c>
+      <c r="BM1" t="inlineStr">
+        <is>
+          <t>product_type_other</t>
+        </is>
+      </c>
+      <c r="BN1" t="inlineStr">
+        <is>
+          <t>prot_flag</t>
+        </is>
+      </c>
+      <c r="BO1" t="inlineStr">
+        <is>
+          <t>prot_data_other</t>
+        </is>
+      </c>
+      <c r="BP1" t="inlineStr">
+        <is>
+          <t>prot_release_date</t>
+        </is>
+      </c>
+      <c r="BQ1" t="inlineStr">
+        <is>
+          <t>availability</t>
+        </is>
+      </c>
+      <c r="BR1" t="inlineStr">
+        <is>
+          <t>subject_category_code</t>
+        </is>
+      </c>
+      <c r="BS1" t="inlineStr">
+        <is>
+          <t>subject_category_code_legacy</t>
+        </is>
+      </c>
+      <c r="BT1" t="inlineStr">
+        <is>
+          <t>related_identifiers</t>
+        </is>
+      </c>
+      <c r="BU1" t="inlineStr">
+        <is>
+          <t>released_to_osti_date</t>
+        </is>
+      </c>
+      <c r="BV1" t="inlineStr">
+        <is>
+          <t>releasing_official_comments</t>
+        </is>
+      </c>
+      <c r="BW1" t="inlineStr">
+        <is>
+          <t>report_period_end_date</t>
+        </is>
+      </c>
+      <c r="BX1" t="inlineStr">
+        <is>
+          <t>report_period_start_date</t>
+        </is>
+      </c>
+      <c r="BY1" t="inlineStr">
+        <is>
+          <t>report_types</t>
+        </is>
+      </c>
+      <c r="BZ1" t="inlineStr">
+        <is>
+          <t>report_type_other</t>
+        </is>
+      </c>
+      <c r="CA1" t="inlineStr">
+        <is>
+          <t>sbiz_flag</t>
+        </is>
+      </c>
+      <c r="CB1" t="inlineStr">
+        <is>
+          <t>sbiz_phase</t>
+        </is>
+      </c>
+      <c r="CC1" t="inlineStr">
+        <is>
+          <t>sbiz_previous_contract_number</t>
+        </is>
+      </c>
+      <c r="CD1" t="inlineStr">
+        <is>
+          <t>sbiz_release_date</t>
+        </is>
+      </c>
+      <c r="CE1" t="inlineStr">
+        <is>
+          <t>site_ownership_code</t>
+        </is>
+      </c>
+      <c r="CF1" t="inlineStr">
+        <is>
+          <t>site_unique_id</t>
+        </is>
+      </c>
+      <c r="CG1" t="inlineStr">
+        <is>
+          <t>site_url</t>
+        </is>
+      </c>
+      <c r="CH1" t="inlineStr">
+        <is>
+          <t>source_input_type</t>
+        </is>
+      </c>
+      <c r="CI1" t="inlineStr">
+        <is>
+          <t>source_edit_type</t>
+        </is>
+      </c>
+      <c r="CJ1" t="inlineStr">
+        <is>
+          <t>geolocations</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation sqref="I2:I1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"R,SA,SR,SO,SF,SX,SV,X,D"</formula1>
+    </dataValidation>
+    <dataValidation sqref="J2:J1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"UNL,OPN,CPY,OUO,PROT,PDOUO,ECI,PDSH,USO,LRD,NAT,NNPI,INTL,PROP,PAT,OTHR,CUI"</formula1>
+    </dataValidation>
+    <dataValidation sqref="R2:R1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"DOE_LAB,DOE_GRANT,CHORUS"</formula1>
+    </dataValidation>
+    <dataValidation sqref="BL2:BL1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"AR,B,CO,DA,FS,JA,MI,OT,P,PD,SM,TD,TR,PA"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -803,7 +1511,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -864,7 +1572,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -903,4 +1611,444 @@
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>relation</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ARK,arXiv,bibcode,DOI,EAN13,EISSN,IGSN,ISBN,ISSN,ISTC,Handle,LISSN,LSID,OTHER,PMCID,PMID,PURL,UPC,URI,URL,URN,UUID,w3id"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>points</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"POINT,BOX,POLYGON"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>latitude</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>longitude</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"AUTH_REV,CN_DOE,CN_NONDOE,CODEN,DOE_DOCKET,EDB,ETDE_RN,INIS_RN,ISBN,ISSN,LEGACY,NSA,OPN_ACC,OTHER_ID,PATENT,PROJ_ID,PROP_REV,REF,REL_TRN,RN,TRN,TVI,USER_VER,WORK_AUTH,WORK_PROP"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>audit_date</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>messages</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>media_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>revision</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>access_limitations</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>osti_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>added_by</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>document_page_count</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>mime_type</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>media_title</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>media_location</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>media_source</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>date_added</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>date_updated</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>date_valid_end</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>files</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"UNL,OPN,CPY,OUO,PROT,PDOUO,ECI,PDSH,USO,LRD,NAT,NNPI,INTL,PROP,PAT,OTHR,CUI"</formula1>
+    </dataValidation>
+    <dataValidation sqref="J2:J1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"L,O"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:X1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>media_file_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>media_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>checksum</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>revision</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>parent_media_file_id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>media_type</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>url_type</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>mime_type</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>added_by_user_id</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>media_source</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>file_size_bytes</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>duration_seconds</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>document_page_count</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>subtitle_tracks</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>video_tracks</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>pdf_version</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>pdfa_conformance</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>pdfa_part</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>pdfua_part</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>processing_exceptions</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>date_file_added</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>date_file_updated</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"L,O"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>